<commit_message>
Lunchtime Friday: Commiting changes from friday.
</commit_message>
<xml_diff>
--- a/q0_modified.xlsx
+++ b/q0_modified.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Per\Dropbox\Pers dropbox\F\Projektarbete15\oil\Matlab Project Shale Oil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Per\Documents\GitHub\matlabTightOil\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>mean</t>
   </si>
@@ -59,6 +59,21 @@
   </si>
   <si>
     <t>sum:</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>median of 2011-2014</t>
+  </si>
+  <si>
+    <t>mean of mean 2011-2014</t>
+  </si>
+  <si>
+    <t>mean of mean 2010-2014</t>
+  </si>
+  <si>
+    <t>median of 2010-2014</t>
   </si>
 </sst>
 </file>
@@ -156,7 +171,6 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +180,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7309,11 +7326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1529181328"/>
-        <c:axId val="-1529184048"/>
+        <c:axId val="-334595056"/>
+        <c:axId val="-334594512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1529181328"/>
+        <c:axId val="-334595056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7355,7 +7372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1529184048"/>
+        <c:crossAx val="-334594512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7363,7 +7380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1529184048"/>
+        <c:axId val="-334594512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7414,7 +7431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1529181328"/>
+        <c:crossAx val="-334595056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7586,7 +7603,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Peak prod (bpd)'!$K$6:$L$6</c:f>
+              <c:f>'Peak prod (bpd)'!$K$9:$L$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7607,7 +7624,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$J$8:$J$37</c:f>
+              <c:f>'Peak prod (bpd)'!$J$11:$J$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -7706,7 +7723,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$L$8:$L$37</c:f>
+              <c:f>'Peak prod (bpd)'!$L$11:$L$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
@@ -7809,7 +7826,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Peak prod (bpd)'!$M$6:$N$6</c:f>
+              <c:f>'Peak prod (bpd)'!$M$9:$N$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7830,7 +7847,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$J$8:$J$37</c:f>
+              <c:f>'Peak prod (bpd)'!$J$11:$J$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -7929,7 +7946,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$N$8:$N$37</c:f>
+              <c:f>'Peak prod (bpd)'!$N$11:$N$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8032,7 +8049,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Peak prod (bpd)'!$O$6:$P$6</c:f>
+              <c:f>'Peak prod (bpd)'!$O$9:$P$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8053,7 +8070,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$J$8:$J$37</c:f>
+              <c:f>'Peak prod (bpd)'!$J$11:$J$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8152,7 +8169,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$P$8:$P$37</c:f>
+              <c:f>'Peak prod (bpd)'!$P$11:$P$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8255,7 +8272,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Peak prod (bpd)'!$Q$6:$R$6</c:f>
+              <c:f>'Peak prod (bpd)'!$Q$9:$R$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8276,7 +8293,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$J$8:$J$37</c:f>
+              <c:f>'Peak prod (bpd)'!$J$11:$J$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8375,7 +8392,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$R$8:$R$37</c:f>
+              <c:f>'Peak prod (bpd)'!$R$11:$R$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8478,7 +8495,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Peak prod (bpd)'!$S$6:$T$6</c:f>
+              <c:f>'Peak prod (bpd)'!$S$9:$T$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8499,7 +8516,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$J$8:$J$37</c:f>
+              <c:f>'Peak prod (bpd)'!$J$11:$J$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8598,7 +8615,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Peak prod (bpd)'!$T$8:$T$37</c:f>
+              <c:f>'Peak prod (bpd)'!$T$11:$T$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8706,11 +8723,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1529184592"/>
-        <c:axId val="-1529182960"/>
+        <c:axId val="-668789696"/>
+        <c:axId val="-254812112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1529184592"/>
+        <c:axId val="-668789696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8814,7 +8831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1529182960"/>
+        <c:crossAx val="-254812112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8822,7 +8839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1529182960"/>
+        <c:axId val="-254812112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8929,7 +8946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1529184592"/>
+        <c:crossAx val="-668789696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -39257,18 +39274,19 @@
   <dimension ref="A1:T927"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="8" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
     <col min="13" max="13" width="8.42578125" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="10.140625" customWidth="1"/>
     <col min="19" max="19" width="8.42578125" customWidth="1"/>
     <col min="20" max="20" width="10.85546875" customWidth="1"/>
@@ -39402,13 +39420,14 @@
         <f>AVERAGE(E2:E480)</f>
         <v>539.22194068693386</v>
       </c>
-      <c r="P3" s="16">
+      <c r="O3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="3">
         <f>AVERAGE(H3:L3)</f>
         <v>487.27307312309847</v>
-      </c>
-      <c r="Q3" s="16">
-        <f>AVERAGE(I3:L3)</f>
-        <v>514.07918386962649</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -39433,27 +39452,36 @@
         <v>568.01095890410954</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H4" s="3">
-        <f>MIN(A2:A65)</f>
-        <v>23.408219178082192</v>
-      </c>
-      <c r="I4" s="17">
-        <f>MIN(B2:B287)</f>
-        <v>0.13150684931506848</v>
+        <f>MEDIAN(A2:A65)</f>
+        <v>242.41643835616438</v>
+      </c>
+      <c r="I4" s="3">
+        <f>MEDIAN(B2:B287)</f>
+        <v>482.05479452054794</v>
       </c>
       <c r="J4" s="3">
-        <f>MIN(C2:C557)</f>
-        <v>1.5123287671232877</v>
-      </c>
-      <c r="K4" s="17">
-        <f>MIN(D2:D927)</f>
-        <v>0.19726027397260273</v>
-      </c>
-      <c r="L4" s="17">
-        <f>MIN(E2:E480)</f>
-        <v>0.32876712328767121</v>
+        <f>MEDIAN(C2:C557)</f>
+        <v>465.81369863013697</v>
+      </c>
+      <c r="K4" s="3">
+        <f>MEDIAN(D2:D927)</f>
+        <v>454.86575342465756</v>
+      </c>
+      <c r="L4" s="3">
+        <f>MEDIAN(E2:E480)</f>
+        <v>481.67671232876711</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="3">
+        <f>AVERAGE(I3:L3)</f>
+        <v>514.07918386962649</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -39478,27 +39506,36 @@
         <v>884.44931506849309</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3">
-        <f>MAX(A2:A65)</f>
-        <v>1816.4383561643835</v>
-      </c>
-      <c r="I5" s="3">
-        <f>MAX(B2:B287)</f>
-        <v>1691.4739726027397</v>
+        <f>MIN(A2:A65)</f>
+        <v>23.408219178082192</v>
+      </c>
+      <c r="I5" s="16">
+        <f>MIN(B2:B287)</f>
+        <v>0.13150684931506848</v>
       </c>
       <c r="J5" s="3">
-        <f>MAX(C2:C557)</f>
-        <v>2860.9643835616439</v>
-      </c>
-      <c r="K5" s="3">
-        <f>MAX(D2:D927)</f>
-        <v>2440.1424657534244</v>
-      </c>
-      <c r="L5" s="3">
-        <f>MAX(E2:E480)</f>
-        <v>3643.7260273972602</v>
+        <f>MIN(C2:C557)</f>
+        <v>1.5123287671232877</v>
+      </c>
+      <c r="K5" s="16">
+        <f>MIN(D2:D927)</f>
+        <v>0.19726027397260273</v>
+      </c>
+      <c r="L5" s="16">
+        <f>MIN(E2:E480)</f>
+        <v>0.32876712328767121</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="3">
+        <f>MEDIAN(A2:A65,B2:B287,C2:C557,D2:D927)</f>
+        <v>456.13150684931509</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -39522,26 +39559,38 @@
         <f>'Peak prod (bpm)'!E6/(365/12)</f>
         <v>850.94794520547941</v>
       </c>
-      <c r="K6" s="18">
-        <v>2010</v>
-      </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="19">
-        <v>2011</v>
-      </c>
-      <c r="N6" s="19"/>
-      <c r="O6" s="20">
-        <v>2012</v>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <f>MAX(A2:A65)</f>
+        <v>1816.4383561643835</v>
+      </c>
+      <c r="I6" s="3">
+        <f>MAX(B2:B287)</f>
+        <v>1691.4739726027397</v>
+      </c>
+      <c r="J6" s="3">
+        <f>MAX(C2:C557)</f>
+        <v>2860.9643835616439</v>
+      </c>
+      <c r="K6" s="3">
+        <f>MAX(D2:D927)</f>
+        <v>2440.1424657534244</v>
+      </c>
+      <c r="L6" s="3">
+        <f>MAX(E2:E480)</f>
+        <v>3643.7260273972602</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="P6" s="20"/>
-      <c r="Q6" s="18">
-        <v>2013</v>
-      </c>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18">
-        <v>2014</v>
-      </c>
-      <c r="T6" s="18"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="3">
+        <f>MEDIAN(B2:B287,C2:C557,D2:D927)</f>
+        <v>462.31232876712329</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -39564,48 +39613,6 @@
         <f>'Peak prod (bpm)'!E7/(365/12)</f>
         <v>454.38904109589038</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="T7" s="10" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -39628,59 +39635,6 @@
         <f>'Peak prod (bpm)'!E8/(365/12)</f>
         <v>506.36712328767123</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>100</v>
-      </c>
-      <c r="J8">
-        <f>H8+(I8-H8)/2</f>
-        <v>50</v>
-      </c>
-      <c r="K8" s="5">
-        <f>COUNTIFS($A$2:$A$65,"&gt;="&amp;H8,$A$2:$A$65,"&lt;="&amp;I8)</f>
-        <v>9</v>
-      </c>
-      <c r="L8" s="12">
-        <f>K8/$K$38</f>
-        <v>0.140625</v>
-      </c>
-      <c r="M8" s="6">
-        <f>COUNTIFS($B$2:$B$287,"&gt;="&amp;H8,$B$2:$B$287,"&lt;="&amp;I8)</f>
-        <v>19</v>
-      </c>
-      <c r="N8" s="13">
-        <f>M8/$M$38</f>
-        <v>6.6433566433566432E-2</v>
-      </c>
-      <c r="O8" s="4">
-        <f>COUNTIFS($C$2:$C$557,"&gt;="&amp;H8,$C$2:$C$557,"&lt;="&amp;I8)</f>
-        <v>16</v>
-      </c>
-      <c r="P8" s="14">
-        <f>O8/$O$38</f>
-        <v>2.8776978417266189E-2</v>
-      </c>
-      <c r="Q8" s="5">
-        <f>COUNTIFS($D$2:$D$927,"&gt;="&amp;H8,$D$2:$D$927,"&lt;="&amp;I8)</f>
-        <v>43</v>
-      </c>
-      <c r="R8" s="15">
-        <f>Q8/$Q$38</f>
-        <v>4.6436285097192227E-2</v>
-      </c>
-      <c r="S8" s="5">
-        <f>COUNTIFS($D$2:$D$480,"&gt;="&amp;H8,$D$2:$D$480,"&lt;="&amp;I8)</f>
-        <v>0</v>
-      </c>
-      <c r="T8" s="13">
-        <f>S8/$S$38</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -39703,61 +39657,26 @@
         <f>'Peak prod (bpm)'!E9/(365/12)</f>
         <v>690.57534246575335</v>
       </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
-        <f>I8</f>
-        <v>100</v>
-      </c>
-      <c r="I9">
-        <f>H9+100</f>
-        <v>200</v>
-      </c>
-      <c r="J9">
-        <f t="shared" ref="J9:J37" si="0">H9+(I9-H9)/2</f>
-        <v>150</v>
-      </c>
-      <c r="K9" s="5">
-        <f>COUNTIFS($A$2:$A$65,"&gt;="&amp;H9,$A$2:$A$65,"&lt;="&amp;I9)</f>
-        <v>21</v>
-      </c>
-      <c r="L9" s="12">
-        <f t="shared" ref="L9:L37" si="1">K9/$K$38</f>
-        <v>0.328125</v>
-      </c>
-      <c r="M9" s="6">
-        <f t="shared" ref="M9:M37" si="2">COUNTIFS($B$2:$B$287,"&gt;="&amp;H9,$B$2:$B$287,"&lt;="&amp;I9)</f>
-        <v>28</v>
-      </c>
-      <c r="N9" s="13">
-        <f t="shared" ref="N9:N37" si="3">M9/$M$38</f>
-        <v>9.7902097902097904E-2</v>
-      </c>
-      <c r="O9" s="4">
-        <f t="shared" ref="O9:O37" si="4">COUNTIFS($C$2:$C$557,"&gt;="&amp;H9,$C$2:$C$557,"&lt;="&amp;I9)</f>
-        <v>37</v>
-      </c>
-      <c r="P9" s="14">
-        <f t="shared" ref="P9:P37" si="5">O9/$O$38</f>
-        <v>6.654676258992806E-2</v>
-      </c>
-      <c r="Q9" s="5">
-        <f t="shared" ref="Q9:Q37" si="6">COUNTIFS($D$2:$D$927,"&gt;="&amp;H9,$D$2:$D$927,"&lt;="&amp;I9)</f>
-        <v>52</v>
-      </c>
-      <c r="R9" s="15">
-        <f t="shared" ref="R9:R37" si="7">Q9/$Q$38</f>
-        <v>5.6155507559395246E-2</v>
-      </c>
-      <c r="S9" s="5">
-        <f t="shared" ref="S9:S37" si="8">COUNTIFS($D$2:$D$480,"&gt;="&amp;H9,$D$2:$D$480,"&lt;="&amp;I9)</f>
-        <v>11</v>
-      </c>
-      <c r="T9" s="13">
-        <f t="shared" ref="T9:T37" si="9">S9/$S$38</f>
-        <v>2.2964509394572025E-2</v>
-      </c>
+      <c r="K9" s="17">
+        <v>2010</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18">
+        <v>2011</v>
+      </c>
+      <c r="N9" s="18"/>
+      <c r="O9" s="19">
+        <v>2012</v>
+      </c>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="17">
+        <v>2013</v>
+      </c>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17">
+        <v>2014</v>
+      </c>
+      <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -39780,60 +39699,47 @@
         <f>'Peak prod (bpm)'!E10/(365/12)</f>
         <v>741.99452054794517</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H10">
-        <f t="shared" ref="H10:H37" si="10">I9</f>
-        <v>200</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ref="I10:I37" si="11">H10+100</f>
-        <v>300</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="K10" s="5">
-        <f>COUNTIFS($A$2:$A$65,"&gt;="&amp;H10,$A$2:$A$65,"&lt;="&amp;I10)</f>
+      <c r="H10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="12">
-        <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="M10" s="6">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="N10" s="13">
-        <f t="shared" si="3"/>
-        <v>0.1048951048951049</v>
-      </c>
-      <c r="O10" s="4">
-        <f t="shared" si="4"/>
-        <v>71</v>
-      </c>
-      <c r="P10" s="14">
-        <f t="shared" si="5"/>
-        <v>0.12769784172661872</v>
-      </c>
-      <c r="Q10" s="5">
-        <f t="shared" si="6"/>
-        <v>94</v>
-      </c>
-      <c r="R10" s="15">
-        <f t="shared" si="7"/>
-        <v>0.10151187904967603</v>
-      </c>
-      <c r="S10" s="5">
-        <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="T10" s="13">
-        <f t="shared" si="9"/>
-        <v>0.10438413361169102</v>
+      <c r="J10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -39858,59 +39764,57 @@
         <v>1259.7041095890411</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <f t="shared" si="10"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="11"/>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
-        <v>350</v>
+        <f>H11+(I11-H11)/2</f>
+        <v>50</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" ref="K11:K37" si="12">COUNTIFS($A$2:$A$65,"&gt;="&amp;H11,$A$2:$A$65,"&lt;="&amp;I11)</f>
-        <v>5</v>
+        <f>COUNTIFS($A$2:$A$65,"&gt;="&amp;H11,$A$2:$A$65,"&lt;="&amp;I11)</f>
+        <v>9</v>
       </c>
       <c r="L11" s="12">
-        <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
+        <f>K11/$K$41</f>
+        <v>0.140625</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" si="2"/>
-        <v>39</v>
+        <f>COUNTIFS($B$2:$B$287,"&gt;="&amp;H11,$B$2:$B$287,"&lt;="&amp;I11)</f>
+        <v>19</v>
       </c>
       <c r="N11" s="13">
-        <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
+        <f>M11/$M$41</f>
+        <v>6.6433566433566432E-2</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="4"/>
-        <v>91</v>
+        <f>COUNTIFS($C$2:$C$557,"&gt;="&amp;H11,$C$2:$C$557,"&lt;="&amp;I11)</f>
+        <v>16</v>
       </c>
       <c r="P11" s="14">
-        <f t="shared" si="5"/>
-        <v>0.16366906474820145</v>
+        <f>O11/$O$41</f>
+        <v>2.8776978417266189E-2</v>
       </c>
       <c r="Q11" s="5">
-        <f t="shared" si="6"/>
-        <v>167</v>
+        <f>COUNTIFS($D$2:$D$927,"&gt;="&amp;H11,$D$2:$D$927,"&lt;="&amp;I11)</f>
+        <v>43</v>
       </c>
       <c r="R11" s="15">
-        <f t="shared" si="7"/>
-        <v>0.18034557235421167</v>
+        <f>Q11/$Q$41</f>
+        <v>4.6436285097192227E-2</v>
       </c>
       <c r="S11" s="5">
-        <f t="shared" si="8"/>
-        <v>96</v>
+        <f>COUNTIFS($D$2:$D$480,"&gt;="&amp;H11,$D$2:$D$480,"&lt;="&amp;I11)</f>
+        <v>0</v>
       </c>
       <c r="T11" s="13">
-        <f t="shared" si="9"/>
-        <v>0.20041753653444677</v>
+        <f>S11/$S$41</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -39935,59 +39839,59 @@
         <v>707.96712328767126</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="10"/>
-        <v>400</v>
+        <f>I11</f>
+        <v>100</v>
       </c>
       <c r="I12">
-        <f t="shared" si="11"/>
-        <v>500</v>
+        <f>H12+100</f>
+        <v>200</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
-        <v>450</v>
+        <f t="shared" ref="J12:J40" si="0">H12+(I12-H12)/2</f>
+        <v>150</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="12"/>
-        <v>7</v>
+        <f>COUNTIFS($A$2:$A$65,"&gt;="&amp;H12,$A$2:$A$65,"&lt;="&amp;I12)</f>
+        <v>21</v>
       </c>
       <c r="L12" s="12">
-        <f t="shared" si="1"/>
-        <v>0.109375</v>
+        <f>K12/$K$41</f>
+        <v>0.328125</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" ref="M12:M40" si="1">COUNTIFS($B$2:$B$287,"&gt;="&amp;H12,$B$2:$B$287,"&lt;="&amp;I12)</f>
+        <v>28</v>
       </c>
       <c r="N12" s="13">
-        <f t="shared" si="3"/>
-        <v>0.11188811188811189</v>
+        <f>M12/$M$41</f>
+        <v>9.7902097902097904E-2</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="4"/>
-        <v>94</v>
+        <f t="shared" ref="O12:O40" si="2">COUNTIFS($C$2:$C$557,"&gt;="&amp;H12,$C$2:$C$557,"&lt;="&amp;I12)</f>
+        <v>37</v>
       </c>
       <c r="P12" s="14">
-        <f t="shared" si="5"/>
-        <v>0.16906474820143885</v>
+        <f>O12/$O$41</f>
+        <v>6.654676258992806E-2</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" si="6"/>
-        <v>179</v>
+        <f t="shared" ref="Q12:Q40" si="3">COUNTIFS($D$2:$D$927,"&gt;="&amp;H12,$D$2:$D$927,"&lt;="&amp;I12)</f>
+        <v>52</v>
       </c>
       <c r="R12" s="15">
-        <f t="shared" si="7"/>
-        <v>0.19330453563714903</v>
+        <f>Q12/$Q$41</f>
+        <v>5.6155507559395246E-2</v>
       </c>
       <c r="S12" s="5">
-        <f t="shared" si="8"/>
-        <v>105</v>
+        <f t="shared" ref="S12:S40" si="4">COUNTIFS($D$2:$D$480,"&gt;="&amp;H12,$D$2:$D$480,"&lt;="&amp;I12)</f>
+        <v>11</v>
       </c>
       <c r="T12" s="13">
-        <f t="shared" si="9"/>
-        <v>0.21920668058455114</v>
+        <f>S12/$S$41</f>
+        <v>2.2964509394572025E-2</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -40012,59 +39916,59 @@
         <v>1321.9397260273972</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <f t="shared" si="10"/>
-        <v>500</v>
+        <f t="shared" ref="H13:H40" si="5">I12</f>
+        <v>200</v>
       </c>
       <c r="I13">
-        <f t="shared" si="11"/>
-        <v>600</v>
+        <f t="shared" ref="I13:I40" si="6">H13+100</f>
+        <v>300</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>250</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($A$2:$A$65,"&gt;="&amp;H13,$A$2:$A$65,"&lt;="&amp;I13)</f>
         <v>5</v>
       </c>
       <c r="L13" s="12">
+        <f>K13/$K$41</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="M13" s="6">
         <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="M13" s="6">
+        <v>30</v>
+      </c>
+      <c r="N13" s="13">
+        <f>M13/$M$41</f>
+        <v>0.1048951048951049</v>
+      </c>
+      <c r="O13" s="4">
         <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="N13" s="13">
+        <v>71</v>
+      </c>
+      <c r="P13" s="14">
+        <f>O13/$O$41</f>
+        <v>0.12769784172661872</v>
+      </c>
+      <c r="Q13" s="5">
         <f t="shared" si="3"/>
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="O13" s="4">
+        <v>94</v>
+      </c>
+      <c r="R13" s="15">
+        <f>Q13/$Q$41</f>
+        <v>0.10151187904967603</v>
+      </c>
+      <c r="S13" s="5">
         <f t="shared" si="4"/>
-        <v>77</v>
-      </c>
-      <c r="P13" s="14">
-        <f t="shared" si="5"/>
-        <v>0.13848920863309352</v>
-      </c>
-      <c r="Q13" s="5">
-        <f t="shared" si="6"/>
-        <v>132</v>
-      </c>
-      <c r="R13" s="15">
-        <f t="shared" si="7"/>
-        <v>0.14254859611231102</v>
-      </c>
-      <c r="S13" s="5">
-        <f t="shared" si="8"/>
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="T13" s="13">
-        <f t="shared" si="9"/>
-        <v>0.15866388308977036</v>
+        <f>S13/$S$41</f>
+        <v>0.10438413361169102</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -40089,59 +39993,59 @@
         <v>441.66575342465751</v>
       </c>
       <c r="G14">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <f t="shared" si="10"/>
-        <v>600</v>
+        <f t="shared" si="5"/>
+        <v>300</v>
       </c>
       <c r="I14">
-        <f t="shared" si="11"/>
-        <v>700</v>
+        <f t="shared" si="6"/>
+        <v>400</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>650</v>
+        <v>350</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="12"/>
-        <v>3</v>
+        <f t="shared" ref="K14:K40" si="7">COUNTIFS($A$2:$A$65,"&gt;="&amp;H14,$A$2:$A$65,"&lt;="&amp;I14)</f>
+        <v>5</v>
       </c>
       <c r="L14" s="12">
+        <f>K14/$K$41</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="M14" s="6">
         <f t="shared" si="1"/>
-        <v>4.6875E-2</v>
-      </c>
-      <c r="M14" s="6">
+        <v>39</v>
+      </c>
+      <c r="N14" s="13">
+        <f>M14/$M$41</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="O14" s="4">
         <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="N14" s="13">
+        <v>91</v>
+      </c>
+      <c r="P14" s="14">
+        <f>O14/$O$41</f>
+        <v>0.16366906474820145</v>
+      </c>
+      <c r="Q14" s="5">
         <f t="shared" si="3"/>
-        <v>0.11188811188811189</v>
-      </c>
-      <c r="O14" s="4">
+        <v>167</v>
+      </c>
+      <c r="R14" s="15">
+        <f>Q14/$Q$41</f>
+        <v>0.18034557235421167</v>
+      </c>
+      <c r="S14" s="5">
         <f t="shared" si="4"/>
-        <v>49</v>
-      </c>
-      <c r="P14" s="14">
-        <f t="shared" si="5"/>
-        <v>8.8129496402877691E-2</v>
-      </c>
-      <c r="Q14" s="5">
-        <f t="shared" si="6"/>
-        <v>78</v>
-      </c>
-      <c r="R14" s="15">
-        <f t="shared" si="7"/>
-        <v>8.4233261339092869E-2</v>
-      </c>
-      <c r="S14" s="5">
-        <f t="shared" si="8"/>
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="T14" s="13">
-        <f t="shared" si="9"/>
-        <v>9.3945720250521919E-2</v>
+        <f>S14/$S$41</f>
+        <v>0.20041753653444677</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -40166,59 +40070,59 @@
         <v>471.45205479452051</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <f t="shared" si="10"/>
-        <v>700</v>
+        <f t="shared" si="5"/>
+        <v>400</v>
       </c>
       <c r="I15">
-        <f t="shared" si="11"/>
-        <v>800</v>
+        <f t="shared" si="6"/>
+        <v>500</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>750</v>
+        <v>450</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="L15" s="12">
+        <f>K15/$K$41</f>
+        <v>0.109375</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" si="1"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="M15" s="6">
+        <v>32</v>
+      </c>
+      <c r="N15" s="13">
+        <f>M15/$M$41</f>
+        <v>0.11188811188811189</v>
+      </c>
+      <c r="O15" s="4">
         <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="N15" s="13">
+        <v>94</v>
+      </c>
+      <c r="P15" s="14">
+        <f>O15/$O$41</f>
+        <v>0.16906474820143885</v>
+      </c>
+      <c r="Q15" s="5">
         <f t="shared" si="3"/>
-        <v>8.0419580419580416E-2</v>
-      </c>
-      <c r="O15" s="4">
+        <v>179</v>
+      </c>
+      <c r="R15" s="15">
+        <f>Q15/$Q$41</f>
+        <v>0.19330453563714903</v>
+      </c>
+      <c r="S15" s="5">
         <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="P15" s="14">
-        <f t="shared" si="5"/>
-        <v>8.0935251798561147E-2</v>
-      </c>
-      <c r="Q15" s="5">
-        <f t="shared" si="6"/>
-        <v>66</v>
-      </c>
-      <c r="R15" s="15">
-        <f t="shared" si="7"/>
-        <v>7.1274298056155511E-2</v>
-      </c>
-      <c r="S15" s="5">
-        <f t="shared" si="8"/>
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="T15" s="13">
-        <f t="shared" si="9"/>
-        <v>9.6033402922755737E-2</v>
+        <f>S15/$S$41</f>
+        <v>0.21920668058455114</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -40243,59 +40147,59 @@
         <v>1393.4465753424656</v>
       </c>
       <c r="G16">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H16">
-        <f t="shared" si="10"/>
-        <v>800</v>
+        <f t="shared" si="5"/>
+        <v>500</v>
       </c>
       <c r="I16">
-        <f t="shared" si="11"/>
-        <v>900</v>
+        <f t="shared" si="6"/>
+        <v>600</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>850</v>
+        <v>550</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="L16" s="12">
+        <f>K16/$K$41</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="M16" s="6">
         <f t="shared" si="1"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="M16" s="6">
+        <v>39</v>
+      </c>
+      <c r="N16" s="13">
+        <f>M16/$M$41</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="O16" s="4">
         <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="N16" s="13">
+        <v>77</v>
+      </c>
+      <c r="P16" s="14">
+        <f>O16/$O$41</f>
+        <v>0.13848920863309352</v>
+      </c>
+      <c r="Q16" s="5">
         <f t="shared" si="3"/>
-        <v>9.7902097902097904E-2</v>
-      </c>
-      <c r="O16" s="4">
+        <v>132</v>
+      </c>
+      <c r="R16" s="15">
+        <f>Q16/$Q$41</f>
+        <v>0.14254859611231102</v>
+      </c>
+      <c r="S16" s="5">
         <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="P16" s="14">
-        <f t="shared" si="5"/>
-        <v>4.3165467625899283E-2</v>
-      </c>
-      <c r="Q16" s="5">
-        <f t="shared" si="6"/>
-        <v>34</v>
-      </c>
-      <c r="R16" s="15">
-        <f t="shared" si="7"/>
-        <v>3.6717062634989202E-2</v>
-      </c>
-      <c r="S16" s="5">
-        <f t="shared" si="8"/>
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T16" s="13">
-        <f t="shared" si="9"/>
-        <v>4.1753653444676408E-2</v>
+        <f>S16/$S$41</f>
+        <v>0.15866388308977036</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -40320,59 +40224,59 @@
         <v>589.41369863013699</v>
       </c>
       <c r="G17">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H17">
-        <f t="shared" si="10"/>
-        <v>900</v>
+        <f t="shared" si="5"/>
+        <v>600</v>
       </c>
       <c r="I17">
-        <f t="shared" si="11"/>
-        <v>1000</v>
+        <f t="shared" si="6"/>
+        <v>700</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>950</v>
+        <v>650</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>3</v>
       </c>
       <c r="L17" s="12">
+        <f>K17/$K$41</f>
+        <v>4.6875E-2</v>
+      </c>
+      <c r="M17" s="6">
         <f t="shared" si="1"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="M17" s="6">
+        <v>32</v>
+      </c>
+      <c r="N17" s="13">
+        <f>M17/$M$41</f>
+        <v>0.11188811188811189</v>
+      </c>
+      <c r="O17" s="4">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="N17" s="13">
+        <v>49</v>
+      </c>
+      <c r="P17" s="14">
+        <f>O17/$O$41</f>
+        <v>8.8129496402877691E-2</v>
+      </c>
+      <c r="Q17" s="5">
         <f t="shared" si="3"/>
-        <v>3.1468531468531472E-2</v>
-      </c>
-      <c r="O17" s="4">
+        <v>78</v>
+      </c>
+      <c r="R17" s="15">
+        <f>Q17/$Q$41</f>
+        <v>8.4233261339092869E-2</v>
+      </c>
+      <c r="S17" s="5">
         <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-      <c r="P17" s="14">
-        <f t="shared" si="5"/>
-        <v>4.4964028776978415E-2</v>
-      </c>
-      <c r="Q17" s="5">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="R17" s="15">
-        <f t="shared" si="7"/>
-        <v>2.159827213822894E-2</v>
-      </c>
-      <c r="S17" s="5">
-        <f t="shared" si="8"/>
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="T17" s="13">
-        <f t="shared" si="9"/>
-        <v>1.6701461377870562E-2</v>
+        <f>S17/$S$41</f>
+        <v>9.3945720250521919E-2</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -40397,59 +40301,59 @@
         <v>691.19999999999993</v>
       </c>
       <c r="G18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H18">
-        <f t="shared" si="10"/>
-        <v>1000</v>
+        <f t="shared" si="5"/>
+        <v>700</v>
       </c>
       <c r="I18">
-        <f t="shared" si="11"/>
-        <v>1100</v>
+        <f t="shared" si="6"/>
+        <v>800</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>1050</v>
+        <v>750</v>
       </c>
       <c r="K18" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="L18" s="12">
+        <f>K18/$K$41</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M18" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="6">
+        <v>23</v>
+      </c>
+      <c r="N18" s="13">
+        <f>M18/$M$41</f>
+        <v>8.0419580419580416E-2</v>
+      </c>
+      <c r="O18" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="N18" s="13">
+        <v>45</v>
+      </c>
+      <c r="P18" s="14">
+        <f>O18/$O$41</f>
+        <v>8.0935251798561147E-2</v>
+      </c>
+      <c r="Q18" s="5">
         <f t="shared" si="3"/>
-        <v>1.048951048951049E-2</v>
-      </c>
-      <c r="O18" s="4">
+        <v>66</v>
+      </c>
+      <c r="R18" s="15">
+        <f>Q18/$Q$41</f>
+        <v>7.1274298056155511E-2</v>
+      </c>
+      <c r="S18" s="5">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="P18" s="14">
-        <f t="shared" si="5"/>
-        <v>1.9784172661870502E-2</v>
-      </c>
-      <c r="Q18" s="5">
-        <f t="shared" si="6"/>
-        <v>19</v>
-      </c>
-      <c r="R18" s="15">
-        <f t="shared" si="7"/>
-        <v>2.0518358531317494E-2</v>
-      </c>
-      <c r="S18" s="5">
-        <f t="shared" si="8"/>
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="T18" s="13">
-        <f t="shared" si="9"/>
-        <v>1.4613778705636743E-2</v>
+        <f>S18/$S$41</f>
+        <v>9.6033402922755737E-2</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -40474,59 +40378,59 @@
         <v>583.75890410958903</v>
       </c>
       <c r="G19">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H19">
-        <f t="shared" si="10"/>
-        <v>1100</v>
+        <f t="shared" si="5"/>
+        <v>800</v>
       </c>
       <c r="I19">
-        <f t="shared" si="11"/>
-        <v>1200</v>
+        <f t="shared" si="6"/>
+        <v>900</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>1150</v>
+        <v>850</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="L19" s="12">
+        <f>K19/$K$41</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M19" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="6">
+        <v>28</v>
+      </c>
+      <c r="N19" s="13">
+        <f>M19/$M$41</f>
+        <v>9.7902097902097904E-2</v>
+      </c>
+      <c r="O19" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="13">
+        <v>24</v>
+      </c>
+      <c r="P19" s="14">
+        <f>O19/$O$41</f>
+        <v>4.3165467625899283E-2</v>
+      </c>
+      <c r="Q19" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="4">
+        <v>34</v>
+      </c>
+      <c r="R19" s="15">
+        <f>Q19/$Q$41</f>
+        <v>3.6717062634989202E-2</v>
+      </c>
+      <c r="S19" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="P19" s="14">
-        <f t="shared" si="5"/>
-        <v>1.4388489208633094E-2</v>
-      </c>
-      <c r="Q19" s="5">
-        <f t="shared" si="6"/>
-        <v>17</v>
-      </c>
-      <c r="R19" s="15">
-        <f t="shared" si="7"/>
-        <v>1.8358531317494601E-2</v>
-      </c>
-      <c r="S19" s="5">
-        <f t="shared" si="8"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="T19" s="13">
-        <f t="shared" si="9"/>
-        <v>1.6701461377870562E-2</v>
+        <f>S19/$S$41</f>
+        <v>4.1753653444676408E-2</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -40551,59 +40455,59 @@
         <v>747.94520547945206</v>
       </c>
       <c r="G20">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H20">
-        <f t="shared" si="10"/>
-        <v>1200</v>
+        <f t="shared" si="5"/>
+        <v>900</v>
       </c>
       <c r="I20">
-        <f t="shared" si="11"/>
-        <v>1300</v>
+        <f t="shared" si="6"/>
+        <v>1000</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>1250</v>
+        <v>950</v>
       </c>
       <c r="K20" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="L20" s="12">
+        <f>K20/$K$41</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M20" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="6">
+        <v>9</v>
+      </c>
+      <c r="N20" s="13">
+        <f>M20/$M$41</f>
+        <v>3.1468531468531472E-2</v>
+      </c>
+      <c r="O20" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="N20" s="13">
+        <v>25</v>
+      </c>
+      <c r="P20" s="14">
+        <f>O20/$O$41</f>
+        <v>4.4964028776978415E-2</v>
+      </c>
+      <c r="Q20" s="5">
         <f t="shared" si="3"/>
-        <v>1.048951048951049E-2</v>
-      </c>
-      <c r="O20" s="4">
+        <v>20</v>
+      </c>
+      <c r="R20" s="15">
+        <f>Q20/$Q$41</f>
+        <v>2.159827213822894E-2</v>
+      </c>
+      <c r="S20" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P20" s="14">
-        <f t="shared" si="5"/>
-        <v>1.7985611510791368E-3</v>
-      </c>
-      <c r="Q20" s="5">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="R20" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5593952483801298E-3</v>
-      </c>
-      <c r="S20" s="5">
-        <f t="shared" si="8"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="T20" s="13">
-        <f t="shared" si="9"/>
-        <v>6.2630480167014616E-3</v>
+        <f>S20/$S$41</f>
+        <v>1.6701461377870562E-2</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -40628,59 +40532,59 @@
         <v>863.27671232876708</v>
       </c>
       <c r="G21">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H21">
-        <f t="shared" si="10"/>
-        <v>1300</v>
+        <f t="shared" si="5"/>
+        <v>1000</v>
       </c>
       <c r="I21">
-        <f t="shared" si="11"/>
-        <v>1400</v>
+        <f t="shared" si="6"/>
+        <v>1100</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>1350</v>
+        <v>1050</v>
       </c>
       <c r="K21" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L21" s="12">
+        <f>K21/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="6">
+        <v>3</v>
+      </c>
+      <c r="N21" s="13">
+        <f>M21/$M$41</f>
+        <v>1.048951048951049E-2</v>
+      </c>
+      <c r="O21" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="13">
+        <v>11</v>
+      </c>
+      <c r="P21" s="14">
+        <f>O21/$O$41</f>
+        <v>1.9784172661870502E-2</v>
+      </c>
+      <c r="Q21" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="4">
+        <v>19</v>
+      </c>
+      <c r="R21" s="15">
+        <f>Q21/$Q$41</f>
+        <v>2.0518358531317494E-2</v>
+      </c>
+      <c r="S21" s="5">
         <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="P21" s="14">
-        <f t="shared" si="5"/>
-        <v>3.5971223021582736E-3</v>
-      </c>
-      <c r="Q21" s="5">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="R21" s="15">
-        <f t="shared" si="7"/>
-        <v>1.0799136069114472E-3</v>
-      </c>
-      <c r="S21" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T21" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>S21/$S$41</f>
+        <v>1.4613778705636743E-2</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -40705,59 +40609,59 @@
         <v>956.25205479452052</v>
       </c>
       <c r="G22">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H22">
-        <f t="shared" si="10"/>
-        <v>1400</v>
+        <f t="shared" si="5"/>
+        <v>1100</v>
       </c>
       <c r="I22">
-        <f t="shared" si="11"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1200</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>1450</v>
+        <v>1150</v>
       </c>
       <c r="K22" s="5">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="L22" s="12">
+        <f>K22/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
         <f t="shared" si="1"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="M22" s="6">
+        <v>0</v>
+      </c>
+      <c r="N22" s="13">
+        <f>M22/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="13">
+        <v>8</v>
+      </c>
+      <c r="P22" s="14">
+        <f>O22/$O$41</f>
+        <v>1.4388489208633094E-2</v>
+      </c>
+      <c r="Q22" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="4">
+        <v>17</v>
+      </c>
+      <c r="R22" s="15">
+        <f>Q22/$Q$41</f>
+        <v>1.8358531317494601E-2</v>
+      </c>
+      <c r="S22" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="5">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="R22" s="15">
-        <f t="shared" si="7"/>
-        <v>4.3196544276457886E-3</v>
-      </c>
-      <c r="S22" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T22" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>S22/$S$41</f>
+        <v>1.6701461377870562E-2</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -40782,59 +40686,59 @@
         <v>541.11780821917807</v>
       </c>
       <c r="G23">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H23">
-        <f t="shared" si="10"/>
-        <v>1500</v>
+        <f t="shared" si="5"/>
+        <v>1200</v>
       </c>
       <c r="I23">
-        <f t="shared" si="11"/>
-        <v>1600</v>
+        <f t="shared" si="6"/>
+        <v>1300</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>1550</v>
+        <v>1250</v>
       </c>
       <c r="K23" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="4">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P23" s="14">
-        <f t="shared" si="5"/>
-        <v>1.7985611510791368E-3</v>
-      </c>
-      <c r="Q23" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="L23" s="12">
+        <f>K23/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N23" s="13">
+        <f>M23/$M$41</f>
+        <v>1.048951048951049E-2</v>
+      </c>
+      <c r="O23" s="4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P23" s="14">
+        <f>O23/$O$41</f>
+        <v>1.7985611510791368E-3</v>
+      </c>
+      <c r="Q23" s="5">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="R23" s="15">
+        <f>Q23/$Q$41</f>
+        <v>7.5593952483801298E-3</v>
+      </c>
       <c r="S23" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="T23" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>S23/$S$41</f>
+        <v>6.2630480167014616E-3</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -40859,58 +40763,58 @@
         <v>1286.2027397260274</v>
       </c>
       <c r="G24">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H24">
-        <f t="shared" si="10"/>
-        <v>1600</v>
+        <f t="shared" si="5"/>
+        <v>1300</v>
       </c>
       <c r="I24">
-        <f t="shared" si="11"/>
-        <v>1700</v>
+        <f t="shared" si="6"/>
+        <v>1400</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>1650</v>
+        <v>1350</v>
       </c>
       <c r="K24" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L24" s="12">
+        <f>K24/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M24" s="6">
+      <c r="N24" s="13">
+        <f>M24/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="4">
         <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P24" s="14">
+        <f>O24/$O$41</f>
+        <v>3.5971223021582736E-3</v>
+      </c>
+      <c r="Q24" s="5">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="N24" s="13">
-        <f t="shared" si="3"/>
-        <v>3.4965034965034965E-3</v>
-      </c>
-      <c r="O24" s="4">
+      <c r="R24" s="15">
+        <f>Q24/$Q$41</f>
+        <v>1.0799136069114472E-3</v>
+      </c>
+      <c r="S24" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P24" s="14">
-        <f t="shared" si="5"/>
-        <v>1.7985611510791368E-3</v>
-      </c>
-      <c r="Q24" s="5">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="R24" s="15">
-        <f t="shared" si="7"/>
-        <v>1.0799136069114472E-3</v>
-      </c>
-      <c r="S24" s="5">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T24" s="13">
-        <f t="shared" si="9"/>
+        <f>S24/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -40936,59 +40840,59 @@
         <v>601.64383561643831</v>
       </c>
       <c r="G25">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H25">
-        <f t="shared" si="10"/>
-        <v>1700</v>
+        <f t="shared" si="5"/>
+        <v>1400</v>
       </c>
       <c r="I25">
-        <f t="shared" si="11"/>
-        <v>1800</v>
+        <f t="shared" si="6"/>
+        <v>1500</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>1750</v>
+        <v>1450</v>
       </c>
       <c r="K25" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="L25" s="12">
+        <f>K25/$K$41</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M25" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="6">
+      <c r="N25" s="13">
+        <f>M25/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N25" s="13">
+      <c r="P25" s="14">
+        <f>O25/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="4">
+        <v>4</v>
+      </c>
+      <c r="R25" s="15">
+        <f>Q25/$Q$41</f>
+        <v>4.3196544276457886E-3</v>
+      </c>
+      <c r="S25" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P25" s="14">
-        <f t="shared" si="5"/>
+      <c r="T25" s="13">
+        <f>S25/$S$41</f>
         <v>0</v>
-      </c>
-      <c r="Q25" s="5">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="R25" s="15">
-        <f t="shared" si="7"/>
-        <v>2.1598272138228943E-3</v>
-      </c>
-      <c r="S25" s="5">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="T25" s="13">
-        <f t="shared" si="9"/>
-        <v>2.0876826722338203E-3</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -41013,59 +40917,59 @@
         <v>554.23561643835615</v>
       </c>
       <c r="G26">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H26">
-        <f t="shared" si="10"/>
-        <v>1800</v>
+        <f t="shared" si="5"/>
+        <v>1500</v>
       </c>
       <c r="I26">
-        <f t="shared" si="11"/>
-        <v>1900</v>
+        <f t="shared" si="6"/>
+        <v>1600</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>1850</v>
+        <v>1550</v>
       </c>
       <c r="K26" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <f>K26/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="13">
+        <f>M26/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L26" s="12">
-        <f t="shared" si="1"/>
-        <v>1.5625E-2</v>
-      </c>
-      <c r="M26" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="13">
+      <c r="P26" s="14">
+        <f>O26/$O$41</f>
+        <v>1.7985611510791368E-3</v>
+      </c>
+      <c r="Q26" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O26" s="4">
+      <c r="R26" s="15">
+        <f>Q26/$Q$41</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P26" s="14">
-        <f t="shared" si="5"/>
+      <c r="T26" s="13">
+        <f>S26/$S$41</f>
         <v>0</v>
-      </c>
-      <c r="Q26" s="5">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="R26" s="15">
-        <f t="shared" si="7"/>
-        <v>2.1598272138228943E-3</v>
-      </c>
-      <c r="S26" s="5">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="T26" s="13">
-        <f t="shared" si="9"/>
-        <v>2.0876826722338203E-3</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -41090,58 +40994,58 @@
         <v>976.37260273972595</v>
       </c>
       <c r="G27">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H27">
-        <f>I26</f>
-        <v>1900</v>
+        <f t="shared" si="5"/>
+        <v>1600</v>
       </c>
       <c r="I27">
-        <f>H27+100</f>
-        <v>2000</v>
+        <f t="shared" si="6"/>
+        <v>1700</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>1650</v>
       </c>
       <c r="K27" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L27" s="12">
+        <f>K27/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="6">
+        <v>1</v>
+      </c>
+      <c r="N27" s="13">
+        <f>M27/$M$41</f>
+        <v>3.4965034965034965E-3</v>
+      </c>
+      <c r="O27" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="13">
+        <v>1</v>
+      </c>
+      <c r="P27" s="14">
+        <f>O27/$O$41</f>
+        <v>1.7985611510791368E-3</v>
+      </c>
+      <c r="Q27" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="4">
+        <v>1</v>
+      </c>
+      <c r="R27" s="15">
+        <f>Q27/$Q$41</f>
+        <v>1.0799136069114472E-3</v>
+      </c>
+      <c r="S27" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P27" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="5">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="R27" s="15">
-        <f t="shared" si="7"/>
-        <v>2.1598272138228943E-3</v>
-      </c>
-      <c r="S27" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T27" s="13">
-        <f t="shared" si="9"/>
+        <f>S27/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41167,59 +41071,59 @@
         <v>1037.8520547945204</v>
       </c>
       <c r="G28">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H28">
-        <f t="shared" si="10"/>
-        <v>2000</v>
+        <f t="shared" si="5"/>
+        <v>1700</v>
       </c>
       <c r="I28">
-        <f t="shared" si="11"/>
-        <v>2100</v>
+        <f t="shared" si="6"/>
+        <v>1800</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>2050</v>
+        <v>1750</v>
       </c>
       <c r="K28" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L28" s="12">
+        <f>K28/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M28" s="6">
+      <c r="N28" s="13">
+        <f>M28/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N28" s="13">
+      <c r="P28" s="14">
+        <f>O28/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="4">
+        <v>2</v>
+      </c>
+      <c r="R28" s="15">
+        <f>Q28/$Q$41</f>
+        <v>2.1598272138228943E-3</v>
+      </c>
+      <c r="S28" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="P28" s="14">
-        <f t="shared" si="5"/>
-        <v>1.7985611510791368E-3</v>
-      </c>
-      <c r="Q28" s="5">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="R28" s="15">
-        <f t="shared" si="7"/>
-        <v>3.2397408207343412E-3</v>
-      </c>
-      <c r="S28" s="5">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
       <c r="T28" s="13">
-        <f t="shared" si="9"/>
-        <v>4.1753653444676405E-3</v>
+        <f>S28/$S$41</f>
+        <v>2.0876826722338203E-3</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -41244,59 +41148,59 @@
         <v>402.21369863013695</v>
       </c>
       <c r="G29">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H29">
-        <f t="shared" si="10"/>
-        <v>2100</v>
+        <f t="shared" si="5"/>
+        <v>1800</v>
       </c>
       <c r="I29">
-        <f t="shared" si="11"/>
-        <v>2200</v>
+        <f t="shared" si="6"/>
+        <v>1900</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>2150</v>
+        <v>1850</v>
       </c>
       <c r="K29" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="L29" s="12">
+        <f>K29/$K$41</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="M29" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M29" s="6">
+      <c r="N29" s="13">
+        <f>M29/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N29" s="13">
+      <c r="P29" s="14">
+        <f>O29/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="4">
+        <v>2</v>
+      </c>
+      <c r="R29" s="15">
+        <f>Q29/$Q$41</f>
+        <v>2.1598272138228943E-3</v>
+      </c>
+      <c r="S29" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="P29" s="14">
-        <f t="shared" si="5"/>
-        <v>1.7985611510791368E-3</v>
-      </c>
-      <c r="Q29" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R29" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S29" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T29" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>S29/$S$41</f>
+        <v>2.0876826722338203E-3</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -41321,58 +41225,58 @@
         <v>824.25205479452052</v>
       </c>
       <c r="G30">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H30">
-        <f t="shared" si="10"/>
-        <v>2200</v>
+        <f>I29</f>
+        <v>1900</v>
       </c>
       <c r="I30">
-        <f t="shared" si="11"/>
-        <v>2300</v>
+        <f>H30+100</f>
+        <v>2000</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>2250</v>
+        <v>1950</v>
       </c>
       <c r="K30" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L30" s="12">
+        <f>K30/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M30" s="6">
+      <c r="N30" s="13">
+        <f>M30/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N30" s="13">
+      <c r="P30" s="14">
+        <f>O30/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="4">
+        <v>2</v>
+      </c>
+      <c r="R30" s="15">
+        <f>Q30/$Q$41</f>
+        <v>2.1598272138228943E-3</v>
+      </c>
+      <c r="S30" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P30" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="5">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="R30" s="15">
-        <f t="shared" si="7"/>
-        <v>2.1598272138228943E-3</v>
-      </c>
-      <c r="S30" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T30" s="13">
-        <f t="shared" si="9"/>
+        <f>S30/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41398,59 +41302,59 @@
         <v>1692.8876712328768</v>
       </c>
       <c r="G31">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H31">
-        <f t="shared" si="10"/>
-        <v>2300</v>
+        <f t="shared" si="5"/>
+        <v>2000</v>
       </c>
       <c r="I31">
-        <f t="shared" si="11"/>
-        <v>2400</v>
+        <f t="shared" si="6"/>
+        <v>2100</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>2350</v>
+        <v>2050</v>
       </c>
       <c r="K31" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L31" s="12">
+        <f>K31/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M31" s="6">
+      <c r="N31" s="13">
+        <f>M31/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="13">
+        <v>1</v>
+      </c>
+      <c r="P31" s="14">
+        <f>O31/$O$41</f>
+        <v>1.7985611510791368E-3</v>
+      </c>
+      <c r="Q31" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="4">
+        <v>3</v>
+      </c>
+      <c r="R31" s="15">
+        <f>Q31/$Q$41</f>
+        <v>3.2397408207343412E-3</v>
+      </c>
+      <c r="S31" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R31" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S31" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T31" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>S31/$S$41</f>
+        <v>4.1753653444676405E-3</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -41475,58 +41379,58 @@
         <v>369.2712328767123</v>
       </c>
       <c r="G32">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H32">
-        <f t="shared" si="10"/>
-        <v>2400</v>
+        <f t="shared" si="5"/>
+        <v>2100</v>
       </c>
       <c r="I32">
-        <f t="shared" si="11"/>
-        <v>2500</v>
+        <f t="shared" si="6"/>
+        <v>2200</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>2450</v>
+        <v>2150</v>
       </c>
       <c r="K32" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L32" s="12">
+        <f>K32/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M32" s="6">
+      <c r="N32" s="13">
+        <f>M32/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="13">
+        <v>1</v>
+      </c>
+      <c r="P32" s="14">
+        <f>O32/$O$41</f>
+        <v>1.7985611510791368E-3</v>
+      </c>
+      <c r="Q32" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O32" s="4">
+      <c r="R32" s="15">
+        <f>Q32/$Q$41</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P32" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="5">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="R32" s="15">
-        <f t="shared" si="7"/>
-        <v>1.0799136069114472E-3</v>
-      </c>
-      <c r="S32" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T32" s="13">
-        <f t="shared" si="9"/>
+        <f>S32/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41552,58 +41456,58 @@
         <v>278.95890410958901</v>
       </c>
       <c r="G33">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H33">
-        <f t="shared" si="10"/>
-        <v>2500</v>
+        <f t="shared" si="5"/>
+        <v>2200</v>
       </c>
       <c r="I33">
-        <f t="shared" si="11"/>
-        <v>2600</v>
+        <f t="shared" si="6"/>
+        <v>2300</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2550</v>
+        <v>2250</v>
       </c>
       <c r="K33" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L33" s="12">
+        <f>K33/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M33" s="6">
+      <c r="N33" s="13">
+        <f>M33/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N33" s="13">
+      <c r="P33" s="14">
+        <f>O33/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O33" s="4">
+        <v>2</v>
+      </c>
+      <c r="R33" s="15">
+        <f>Q33/$Q$41</f>
+        <v>2.1598272138228943E-3</v>
+      </c>
+      <c r="S33" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P33" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R33" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S33" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T33" s="13">
-        <f t="shared" si="9"/>
+        <f>S33/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41629,58 +41533,58 @@
         <v>790.48767123287666</v>
       </c>
       <c r="G34">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H34">
-        <f t="shared" si="10"/>
-        <v>2600</v>
+        <f t="shared" si="5"/>
+        <v>2300</v>
       </c>
       <c r="I34">
-        <f t="shared" si="11"/>
-        <v>2700</v>
+        <f t="shared" si="6"/>
+        <v>2400</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2650</v>
+        <v>2350</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L34" s="12">
+        <f>K34/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M34" s="6">
+      <c r="N34" s="13">
+        <f>M34/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N34" s="13">
+      <c r="P34" s="14">
+        <f>O34/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O34" s="4">
+      <c r="R34" s="15">
+        <f>Q34/$Q$41</f>
+        <v>0</v>
+      </c>
+      <c r="S34" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P34" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R34" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S34" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T34" s="13">
-        <f t="shared" si="9"/>
+        <f>S34/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41706,58 +41610,58 @@
         <v>349.70958904109585</v>
       </c>
       <c r="G35">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H35">
-        <f t="shared" si="10"/>
-        <v>2700</v>
+        <f t="shared" si="5"/>
+        <v>2400</v>
       </c>
       <c r="I35">
-        <f t="shared" si="11"/>
-        <v>2800</v>
+        <f t="shared" si="6"/>
+        <v>2500</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>2750</v>
+        <v>2450</v>
       </c>
       <c r="K35" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L35" s="12">
+        <f>K35/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M35" s="6">
+      <c r="N35" s="13">
+        <f>M35/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N35" s="13">
+      <c r="P35" s="14">
+        <f>O35/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="4">
+        <v>1</v>
+      </c>
+      <c r="R35" s="15">
+        <f>Q35/$Q$41</f>
+        <v>1.0799136069114472E-3</v>
+      </c>
+      <c r="S35" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P35" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R35" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S35" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T35" s="13">
-        <f t="shared" si="9"/>
+        <f>S35/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41783,58 +41687,58 @@
         <v>693.36986301369859</v>
       </c>
       <c r="G36">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H36">
-        <f t="shared" si="10"/>
-        <v>2800</v>
+        <f t="shared" si="5"/>
+        <v>2500</v>
       </c>
       <c r="I36">
-        <f t="shared" si="11"/>
-        <v>2900</v>
+        <f t="shared" si="6"/>
+        <v>2600</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>2850</v>
+        <v>2550</v>
       </c>
       <c r="K36" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L36" s="12">
+        <f>K36/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M36" s="6">
+      <c r="N36" s="13">
+        <f>M36/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N36" s="13">
+      <c r="P36" s="14">
+        <f>O36/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O36" s="4">
+      <c r="R36" s="15">
+        <f>Q36/$Q$41</f>
+        <v>0</v>
+      </c>
+      <c r="S36" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P36" s="14">
-        <f t="shared" si="5"/>
-        <v>1.7985611510791368E-3</v>
-      </c>
-      <c r="Q36" s="5">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R36" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S36" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T36" s="13">
-        <f t="shared" si="9"/>
+        <f>S36/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41860,58 +41764,58 @@
         <v>462.37808219178078</v>
       </c>
       <c r="G37">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H37">
-        <f t="shared" si="10"/>
-        <v>2900</v>
+        <f t="shared" si="5"/>
+        <v>2600</v>
       </c>
       <c r="I37">
-        <f t="shared" si="11"/>
-        <v>3000</v>
+        <f t="shared" si="6"/>
+        <v>2700</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>2950</v>
+        <v>2650</v>
       </c>
       <c r="K37" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L37" s="12">
+        <f>K37/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M37" s="6">
+      <c r="N37" s="13">
+        <f>M37/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N37" s="13">
+      <c r="P37" s="14">
+        <f>O37/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O37" s="4">
+      <c r="R37" s="15">
+        <f>Q37/$Q$41</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P37" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q37" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R37" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S37" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="T37" s="13">
-        <f t="shared" si="9"/>
+        <f>S37/$S$41</f>
         <v>0</v>
       </c>
     </row>
@@ -41936,27 +41840,60 @@
         <f>'Peak prod (bpm)'!E38/(365/12)</f>
         <v>620.84383561643835</v>
       </c>
+      <c r="G38">
+        <v>28</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="5"/>
+        <v>2700</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="6"/>
+        <v>2800</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>2750</v>
+      </c>
       <c r="K38" s="5">
-        <f>SUM(K8:K37)</f>
-        <v>64</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L38" s="12">
+        <f>K38/$K$41</f>
+        <v>0</v>
       </c>
       <c r="M38" s="6">
-        <f>SUM(M8:M37)</f>
-        <v>286</v>
-      </c>
-      <c r="N38" s="6"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="13">
+        <f>M38/$M$41</f>
+        <v>0</v>
+      </c>
       <c r="O38" s="4">
-        <f>SUM(O8:O37)</f>
-        <v>556</v>
-      </c>
-      <c r="P38" s="4"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="14">
+        <f>O38/$O$41</f>
+        <v>0</v>
+      </c>
       <c r="Q38" s="5">
-        <f>SUM(Q8:Q37)</f>
-        <v>926</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R38" s="15">
+        <f>Q38/$Q$41</f>
+        <v>0</v>
       </c>
       <c r="S38" s="5">
-        <f>SUM(S8:S37)</f>
-        <v>479</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T38" s="13">
+        <f>S38/$S$41</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -41980,6 +41917,61 @@
         <f>'Peak prod (bpm)'!E39/(365/12)</f>
         <v>1467.0246575342464</v>
       </c>
+      <c r="G39">
+        <v>29</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="5"/>
+        <v>2800</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="6"/>
+        <v>2900</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>2850</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="12">
+        <f>K39/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="13">
+        <f>M39/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P39" s="14">
+        <f>O39/$O$41</f>
+        <v>1.7985611510791368E-3</v>
+      </c>
+      <c r="Q39" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="15">
+        <f>Q39/$Q$41</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="13">
+        <f>S39/$S$41</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -42002,6 +41994,61 @@
         <f>'Peak prod (bpm)'!E40/(365/12)</f>
         <v>2270.5643835616438</v>
       </c>
+      <c r="G40">
+        <v>30</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="5"/>
+        <v>2900</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="6"/>
+        <v>3000</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>2950</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
+        <f>K40/$K$41</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="13">
+        <f>M40/$M$41</f>
+        <v>0</v>
+      </c>
+      <c r="O40" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="14">
+        <f>O40/$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="15">
+        <f>Q40/$Q$41</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T40" s="13">
+        <f>S40/$S$41</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -42024,6 +42071,28 @@
         <f>'Peak prod (bpm)'!E41/(365/12)</f>
         <v>364.37260273972601</v>
       </c>
+      <c r="K41" s="5">
+        <f>SUM(K11:K40)</f>
+        <v>64</v>
+      </c>
+      <c r="M41" s="6">
+        <f>SUM(M11:M40)</f>
+        <v>286</v>
+      </c>
+      <c r="N41" s="6"/>
+      <c r="O41" s="4">
+        <f>SUM(O11:O40)</f>
+        <v>556</v>
+      </c>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="5">
+        <f>SUM(Q11:Q40)</f>
+        <v>926</v>
+      </c>
+      <c r="S41" s="5">
+        <f>SUM(S11:S40)</f>
+        <v>479</v>
+      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -52242,15 +52311,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
+  <mergeCells count="9">
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>